<commit_message>
organized and fixxed typos
</commit_message>
<xml_diff>
--- a/results/commons-lang-ratios.xlsx
+++ b/results/commons-lang-ratios.xlsx
@@ -10,7 +10,6 @@
     <sheet name="commons-lang-ratios" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -301,38 +300,8 @@
               <a:rPr lang="en-US" sz="1700" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Average Difference Between Kill Rates of Mutation Operator Pairs in Commons-Lang</a:t>
+              <a:t>Average Difference Between Kill Rates of Mutation Operator Pairs</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1700">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -535,11 +504,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="66309504"/>
-        <c:axId val="66315776"/>
+        <c:axId val="111493504"/>
+        <c:axId val="111495424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66309504"/>
+        <c:axId val="111493504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66315776"/>
+        <c:crossAx val="111495424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -575,7 +544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66315776"/>
+        <c:axId val="111495424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66309504"/>
+        <c:crossAx val="111493504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -989,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K171" sqref="K171"/>
+    <sheetView tabSelected="1" topLeftCell="C171" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T173" sqref="T173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>